<commit_message>
Published state of ETDataset on 29 May 2015
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/transport/transport_car_using_electricity.converter.xlsx
+++ b/nodes_source_analyses/transport/transport_car_using_electricity.converter.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="762"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16140" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="103">
   <si>
     <t>Source</t>
   </si>
@@ -70,9 +70,6 @@
     <t>NL</t>
   </si>
   <si>
-    <t>households_supplied_per_unit</t>
-  </si>
-  <si>
     <t>Definition</t>
   </si>
   <si>
@@ -350,23 +347,53 @@
   </si>
   <si>
     <t>http://refman.et-model.com/publications/1930</t>
+  </si>
+  <si>
+    <r>
+      <t>quintel/etsource@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2740f4510acc9daf24a2cd9283ca953db9a11779</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.000000000000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -834,454 +861,456 @@
   </borders>
   <cellStyleXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="24" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="26" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2239,7 +2268,7 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2257,7 +2286,7 @@
     <row r="2" spans="1:3" ht="20">
       <c r="A2" s="1"/>
       <c r="B2" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="27"/>
     </row>
@@ -2269,28 +2298,28 @@
     <row r="4" spans="1:3">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2306,7 +2335,7 @@
     <row r="9" spans="1:3">
       <c r="A9" s="1"/>
       <c r="B9" s="89" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="90"/>
     </row>
@@ -2318,31 +2347,31 @@
     <row r="11" spans="1:3">
       <c r="A11" s="1"/>
       <c r="B11" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="93" t="s">
         <v>71</v>
-      </c>
-      <c r="C11" s="93" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" thickBot="1">
       <c r="A12" s="1"/>
       <c r="B12" s="91"/>
       <c r="C12" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" thickBot="1">
       <c r="A13" s="1"/>
       <c r="B13" s="91"/>
       <c r="C13" s="94" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1"/>
       <c r="B14" s="91"/>
       <c r="C14" s="92" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2353,61 +2382,64 @@
     <row r="16" spans="1:3">
       <c r="A16" s="1"/>
       <c r="B16" s="91" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="95" t="s">
         <v>76</v>
-      </c>
-      <c r="C16" s="95" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1"/>
       <c r="B17" s="91"/>
       <c r="C17" s="96" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1"/>
       <c r="B18" s="91"/>
       <c r="C18" s="97" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1"/>
       <c r="B19" s="91"/>
       <c r="C19" s="98" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1"/>
       <c r="B20" s="99"/>
       <c r="C20" s="100" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1"/>
       <c r="B21" s="99"/>
       <c r="C21" s="101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1"/>
       <c r="B22" s="99"/>
       <c r="C22" s="102" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="B23" s="99"/>
       <c r="C23" s="103" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:B2">
+    <sortCondition descending="1" ref="A1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2423,11 +2455,9 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:K36"/>
+  <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2451,36 +2481,36 @@
       <c r="G1" s="36"/>
     </row>
     <row r="2" spans="2:11">
-      <c r="B2" s="123" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="125"/>
+      <c r="B2" s="125" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="127"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="126"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="128"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="130"/>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="126"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
-      <c r="E4" s="128"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="130"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="131"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="133"/>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
     </row>
@@ -2501,17 +2531,17 @@
     <row r="8" spans="2:11" s="23" customFormat="1">
       <c r="B8" s="111"/>
       <c r="C8" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="15" t="s">
@@ -2533,7 +2563,7 @@
     <row r="10" spans="2:11" s="23" customFormat="1" ht="16" thickBot="1">
       <c r="B10" s="22"/>
       <c r="C10" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="13"/>
@@ -2546,7 +2576,7 @@
     <row r="11" spans="2:11" s="23" customFormat="1" ht="16" thickBot="1">
       <c r="B11" s="22"/>
       <c r="C11" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>3</v>
@@ -2558,14 +2588,14 @@
       <c r="G11" s="39"/>
       <c r="H11" s="30"/>
       <c r="I11" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="2:11" ht="16" thickBot="1">
       <c r="B12" s="40"/>
       <c r="C12" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>3</v>
@@ -2577,7 +2607,7 @@
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
       <c r="I12" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J12" s="110"/>
       <c r="K12" s="36"/>
@@ -2585,7 +2615,7 @@
     <row r="13" spans="2:11" ht="16" thickBot="1">
       <c r="B13" s="40"/>
       <c r="C13" s="39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>3</v>
@@ -2597,7 +2627,7 @@
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
       <c r="I13" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J13" s="110"/>
       <c r="K13" s="36"/>
@@ -2605,19 +2635,19 @@
     <row r="14" spans="2:11" ht="16" thickBot="1">
       <c r="B14" s="40"/>
       <c r="C14" s="39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="34">
-        <v>0.05</v>
+      <c r="E14" s="41">
+        <v>0</v>
       </c>
       <c r="F14" s="39"/>
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
       <c r="I14" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14" s="110"/>
       <c r="K14" s="36"/>
@@ -2625,19 +2655,19 @@
     <row r="15" spans="2:11" ht="16" thickBot="1">
       <c r="B15" s="40"/>
       <c r="C15" s="39" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="41">
-        <v>0</v>
+      <c r="E15" s="42">
+        <v>1104.9363103000001</v>
       </c>
       <c r="F15" s="39"/>
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
-      <c r="I15" s="34" t="s">
-        <v>38</v>
+      <c r="I15" s="123" t="s">
+        <v>102</v>
       </c>
       <c r="J15" s="110"/>
       <c r="K15" s="36"/>
@@ -2645,19 +2675,19 @@
     <row r="16" spans="2:11" ht="16" thickBot="1">
       <c r="B16" s="40"/>
       <c r="C16" s="39" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="42">
-        <v>408.82643481555903</v>
+      <c r="E16" s="34">
+        <v>0</v>
       </c>
       <c r="F16" s="39"/>
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
       <c r="I16" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J16" s="110"/>
       <c r="K16" s="36"/>
@@ -2677,7 +2707,7 @@
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
       <c r="I17" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17" s="110"/>
       <c r="K17" s="36"/>
@@ -2685,22 +2715,21 @@
     <row r="18" spans="2:11" ht="16" thickBot="1">
       <c r="B18" s="40"/>
       <c r="C18" s="39" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="34">
-        <v>0</v>
+      <c r="E18" s="124">
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="F18" s="39"/>
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
-      <c r="I18" s="34" t="s">
-        <v>38</v>
+      <c r="I18" s="123" t="s">
+        <v>102</v>
       </c>
       <c r="J18" s="110"/>
-      <c r="K18" s="36"/>
     </row>
     <row r="19" spans="2:11" ht="16" thickBot="1">
       <c r="B19" s="40"/>
@@ -2711,13 +2740,13 @@
         <v>3</v>
       </c>
       <c r="E19" s="42">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F19" s="39"/>
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
       <c r="I19" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19" s="110"/>
     </row>
@@ -2729,46 +2758,48 @@
       <c r="D20" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="42">
-        <v>0</v>
+      <c r="E20" s="124">
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="F20" s="39"/>
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
-      <c r="I20" s="34" t="s">
-        <v>38</v>
+      <c r="I20" s="123" t="s">
+        <v>102</v>
       </c>
       <c r="J20" s="110"/>
     </row>
     <row r="21" spans="2:11" ht="16" thickBot="1">
       <c r="B21" s="40"/>
       <c r="C21" s="39" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="42">
-        <v>0.01</v>
+        <v>2</v>
+      </c>
+      <c r="E21" s="41">
+        <v>0.221747873829401</v>
       </c>
       <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
+      <c r="G21" s="68" t="s">
+        <v>42</v>
+      </c>
       <c r="H21" s="39"/>
       <c r="I21" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J21" s="110"/>
     </row>
     <row r="22" spans="2:11" ht="16" thickBot="1">
       <c r="B22" s="40"/>
       <c r="C22" s="39" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="41">
-        <v>0.221747873829401</v>
+        <v>0.78572582355204501</v>
       </c>
       <c r="F22" s="39"/>
       <c r="G22" s="68" t="s">
@@ -2776,20 +2807,20 @@
       </c>
       <c r="H22" s="39"/>
       <c r="I22" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J22" s="110"/>
     </row>
     <row r="23" spans="2:11" ht="16" thickBot="1">
       <c r="B23" s="40"/>
       <c r="C23" s="39" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="41">
-        <v>0.78572582355204501</v>
+        <v>0.28698540649274501</v>
       </c>
       <c r="F23" s="39"/>
       <c r="G23" s="68" t="s">
@@ -2797,7 +2828,7 @@
       </c>
       <c r="H23" s="39"/>
       <c r="I23" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J23" s="110"/>
     </row>
@@ -2810,7 +2841,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="41">
-        <v>0.28698540649274501</v>
+        <v>0.97934745639203202</v>
       </c>
       <c r="F24" s="39"/>
       <c r="G24" s="68" t="s">
@@ -2818,7 +2849,7 @@
       </c>
       <c r="H24" s="39"/>
       <c r="I24" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J24" s="110"/>
     </row>
@@ -2830,43 +2861,35 @@
       <c r="D25" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="41">
-        <v>0.97934745639203202</v>
+      <c r="E25" s="46">
+        <v>1358.90321232822</v>
       </c>
       <c r="F25" s="39"/>
-      <c r="G25" s="68" t="s">
-        <v>46</v>
+      <c r="G25" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="H25" s="39"/>
       <c r="I25" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J25" s="110"/>
     </row>
-    <row r="26" spans="2:11" ht="16" thickBot="1">
+    <row r="26" spans="2:11">
       <c r="B26" s="40"/>
-      <c r="C26" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="46">
-        <v>1358.90321232822</v>
-      </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" s="39"/>
-      <c r="I26" s="34" t="s">
-        <v>38</v>
-      </c>
+      <c r="C26" s="36"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="114"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="110"/>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" ht="16" thickBot="1">
       <c r="B27" s="40"/>
-      <c r="C27" s="36"/>
+      <c r="C27" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="D27" s="113"/>
       <c r="E27" s="114"/>
       <c r="F27" s="36"/>
@@ -2877,15 +2900,24 @@
     </row>
     <row r="28" spans="2:11" ht="16" thickBot="1">
       <c r="B28" s="40"/>
-      <c r="C28" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="113"/>
-      <c r="E28" s="114"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
+      <c r="C28" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="41">
+        <f>'Research data'!H10</f>
+        <v>24900</v>
+      </c>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="39"/>
+      <c r="I28" s="72" t="s">
+        <v>62</v>
+      </c>
       <c r="J28" s="110"/>
     </row>
     <row r="29" spans="2:11" ht="16" thickBot="1">
@@ -2894,66 +2926,57 @@
         <v>33</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="41">
-        <f>'Research data'!H10</f>
-        <v>24900</v>
+        <v>36</v>
+      </c>
+      <c r="E29" s="109">
+        <f>'Research data'!H11</f>
+        <v>180</v>
       </c>
       <c r="F29" s="39"/>
       <c r="G29" s="39" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H29" s="39"/>
       <c r="I29" s="72" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="J29" s="110"/>
     </row>
     <row r="30" spans="2:11" ht="16" thickBot="1">
       <c r="B30" s="40"/>
       <c r="C30" s="39" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="D30" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="42">
+        <v>0.01</v>
+      </c>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="109">
-        <f>'Research data'!H11</f>
-        <v>180</v>
-      </c>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="39"/>
-      <c r="I30" s="72" t="s">
-        <v>99</v>
-      </c>
       <c r="J30" s="110"/>
     </row>
-    <row r="31" spans="2:11" ht="16" thickBot="1">
+    <row r="31" spans="2:11">
       <c r="B31" s="40"/>
-      <c r="C31" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="42">
-        <v>0.01</v>
-      </c>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="34" t="s">
-        <v>38</v>
-      </c>
+      <c r="C31" s="36"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="115"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="74"/>
       <c r="J31" s="110"/>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:11" ht="16" thickBot="1">
       <c r="B32" s="40"/>
-      <c r="C32" s="36"/>
+      <c r="C32" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="D32" s="113"/>
       <c r="E32" s="115"/>
       <c r="F32" s="36"/>
@@ -2964,68 +2987,55 @@
     </row>
     <row r="33" spans="2:10" ht="16" thickBot="1">
       <c r="B33" s="40"/>
-      <c r="C33" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="113"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="110"/>
-    </row>
-    <row r="34" spans="2:10" ht="16" thickBot="1">
-      <c r="B34" s="40"/>
-      <c r="C34" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="21" t="s">
+      <c r="C33" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E33" s="41">
         <f>'Research data'!H7</f>
         <v>15</v>
       </c>
-      <c r="F34" s="39"/>
-      <c r="G34" s="88" t="s">
-        <v>67</v>
-      </c>
-      <c r="H34" s="39"/>
-      <c r="I34" s="120" t="s">
-        <v>64</v>
+      <c r="F33" s="39"/>
+      <c r="G33" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" s="39"/>
+      <c r="I33" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="J33" s="110"/>
+    </row>
+    <row r="34" spans="2:10" ht="16" thickBot="1">
+      <c r="B34" s="116"/>
+      <c r="C34" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="117">
+        <v>0</v>
+      </c>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="118" t="s">
+        <v>37</v>
       </c>
       <c r="J34" s="110"/>
     </row>
-    <row r="35" spans="2:10" ht="16" thickBot="1">
-      <c r="B35" s="116"/>
-      <c r="C35" s="68" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="117">
-        <v>0</v>
-      </c>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="118" t="s">
-        <v>38</v>
-      </c>
-      <c r="J35" s="110"/>
-    </row>
-    <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1">
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="45"/>
+    <row r="35" spans="2:10" ht="15" customHeight="1" thickBot="1">
+      <c r="B35" s="43"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3134,40 +3144,40 @@
     <row r="4" spans="2:20" s="23" customFormat="1">
       <c r="B4" s="22"/>
       <c r="C4" s="104" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="104" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="104"/>
       <c r="H4" s="104" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I4" s="104"/>
       <c r="J4" s="104" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" s="104"/>
       <c r="L4" s="104" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M4" s="104"/>
       <c r="N4" s="104" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O4" s="104"/>
       <c r="P4" s="104" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q4" s="104"/>
       <c r="R4" s="104" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S4" s="104"/>
       <c r="T4" s="104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:20" ht="18" customHeight="1">
@@ -3266,7 +3276,7 @@
     <row r="9" spans="2:20" ht="16" thickBot="1">
       <c r="B9" s="51"/>
       <c r="C9" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -3289,12 +3299,12 @@
     <row r="10" spans="2:20" ht="16" thickBot="1">
       <c r="B10" s="51"/>
       <c r="C10" s="108" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="69" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="106"/>
       <c r="H10" s="57">
@@ -3326,12 +3336,12 @@
     <row r="11" spans="2:20" ht="16" thickBot="1">
       <c r="B11" s="51"/>
       <c r="C11" s="108" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="62"/>
       <c r="E11" s="62"/>
       <c r="F11" s="107" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="105"/>
       <c r="H11" s="63">
@@ -3405,7 +3415,7 @@
     <row r="3" spans="2:10">
       <c r="B3" s="79"/>
       <c r="C3" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
@@ -3429,28 +3439,28 @@
     <row r="5" spans="2:10">
       <c r="B5" s="84"/>
       <c r="C5" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>21</v>
-      </c>
       <c r="I5" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -3468,7 +3478,7 @@
       <c r="B7" s="79"/>
       <c r="C7" s="85"/>
       <c r="D7" s="74" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="74" t="s">
         <v>8</v>
@@ -3476,11 +3486,11 @@
       <c r="F7" s="74"/>
       <c r="G7" s="74"/>
       <c r="H7" s="80" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="74"/>
       <c r="J7" s="53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="2:10">
@@ -3511,7 +3521,7 @@
       <c r="B10" s="79"/>
       <c r="C10" s="86"/>
       <c r="D10" s="74" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="74" t="s">
         <v>8</v>
@@ -3519,11 +3529,11 @@
       <c r="F10" s="74"/>
       <c r="G10" s="74"/>
       <c r="H10" s="80" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" s="74"/>
       <c r="J10" s="75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:10">
@@ -3552,7 +3562,7 @@
       <c r="B13" s="79"/>
       <c r="C13" s="86"/>
       <c r="D13" s="74" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="74" t="s">
         <v>8</v>
@@ -3560,11 +3570,11 @@
       <c r="F13" s="74"/>
       <c r="G13" s="74"/>
       <c r="H13" s="80" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I13" s="74"/>
       <c r="J13" s="74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:10">
@@ -3595,10 +3605,10 @@
       <c r="B16" s="79"/>
       <c r="C16" s="86"/>
       <c r="D16" s="74" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="74" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="74">
         <v>2012</v>
@@ -3608,10 +3618,10 @@
       </c>
       <c r="H16" s="74"/>
       <c r="I16" s="122" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J16" s="121" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -3642,7 +3652,7 @@
       <c r="B19" s="79"/>
       <c r="C19" s="85"/>
       <c r="D19" s="74" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E19" s="74" t="s">
         <v>8</v>
@@ -3655,16 +3665,16 @@
       </c>
       <c r="H19" s="74"/>
       <c r="I19" s="122" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J19" s="74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="79"/>
       <c r="C20" s="85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="74"/>
       <c r="E20" s="74"/>
@@ -3726,11 +3736,11 @@
       <c r="A3" s="23"/>
       <c r="B3" s="111"/>
       <c r="C3" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -3772,7 +3782,7 @@
     <row r="6" spans="1:13">
       <c r="B6" s="79"/>
       <c r="C6" s="74" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="74"/>
       <c r="E6" s="74"/>
@@ -3807,7 +3817,7 @@
         <v>29990</v>
       </c>
       <c r="F8" s="119" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="74"/>
       <c r="H8" s="74"/>
@@ -4100,7 +4110,7 @@
     <row r="29" spans="2:13">
       <c r="B29" s="79"/>
       <c r="C29" s="74" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="74"/>
       <c r="E29" s="74"/>
@@ -4247,7 +4257,7 @@
         <v>24110</v>
       </c>
       <c r="F39" s="119" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G39" s="74"/>
       <c r="H39" s="74"/>
@@ -4498,7 +4508,7 @@
     <row r="57" spans="2:13">
       <c r="B57" s="79"/>
       <c r="C57" s="74" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D57" s="74"/>
       <c r="E57" s="74"/>
@@ -4589,7 +4599,7 @@
         <v>20600</v>
       </c>
       <c r="F63" s="119" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G63" s="74"/>
       <c r="H63" s="74"/>
@@ -4756,7 +4766,7 @@
     <row r="75" spans="2:13">
       <c r="B75" s="79"/>
       <c r="C75" s="119" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D75" s="74"/>
       <c r="E75" s="74"/>
@@ -4772,7 +4782,7 @@
     <row r="76" spans="2:13">
       <c r="B76" s="79"/>
       <c r="C76" s="119" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D76" s="74"/>
       <c r="E76" s="74"/>
@@ -4863,7 +4873,7 @@
         <v>180</v>
       </c>
       <c r="F82" s="119" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G82" s="74"/>
       <c r="H82" s="74"/>
@@ -4946,7 +4956,7 @@
     <row r="88" spans="2:13">
       <c r="B88" s="79"/>
       <c r="C88" s="119" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D88" s="74"/>
       <c r="E88" s="74"/>
@@ -4962,7 +4972,7 @@
     <row r="89" spans="2:13">
       <c r="B89" s="79"/>
       <c r="C89" s="119" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D89" s="74"/>
       <c r="E89" s="74"/>
@@ -4997,7 +5007,7 @@
         <v>15</v>
       </c>
       <c r="F91" s="119" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G91" s="74"/>
       <c r="H91" s="74"/>

</xml_diff>

<commit_message>
Published state of ETDataset on 22 March 2016
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/transport/transport_car_using_electricity.converter.xlsx
+++ b/nodes_source_analyses/transport/transport_car_using_electricity.converter.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="-20" windowWidth="19200" windowHeight="23460" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16100" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="142">
   <si>
     <t>Source</t>
   </si>
@@ -535,6 +535,9 @@
   <si>
     <t>storage_volume</t>
   </si>
+  <si>
+    <t>Hard-coded to 25 kWh, see https://github.com/quintel/etmoses/issues/808#issuecomment-199221082 fro discussion</t>
+  </si>
 </sst>
 </file>
 
@@ -548,12 +551,19 @@
     <numFmt numFmtId="168" formatCode="0.0E+00;\_x0000_"/>
     <numFmt numFmtId="169" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1060,571 +1070,572 @@
   </borders>
   <cellStyleXfs count="296">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="31" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="32" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="296">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2790,9 +2801,7 @@
   </sheetPr>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2816,36 +2825,36 @@
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="2:11">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="166" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="166"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="168"/>
       <c r="F2" s="35"/>
       <c r="G2" s="35"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="167"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="169"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="35"/>
       <c r="G3" s="35"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="167"/>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="169"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="35"/>
       <c r="G4" s="35"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="170"/>
-      <c r="C5" s="171"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="172"/>
+      <c r="B5" s="172"/>
+      <c r="C5" s="173"/>
+      <c r="D5" s="173"/>
+      <c r="E5" s="174"/>
       <c r="F5" s="35"/>
       <c r="G5" s="35"/>
     </row>
@@ -2939,13 +2948,15 @@
         <v>102</v>
       </c>
       <c r="E12" s="149">
-        <f>'Research data'!H8/1000</f>
-        <v>2.0175000000000002E-2</v>
+        <f>0.025</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F12" s="38"/>
       <c r="G12" s="135"/>
       <c r="H12" s="29"/>
-      <c r="I12" s="142"/>
+      <c r="I12" s="175" t="s">
+        <v>141</v>
+      </c>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="2:11" s="22" customFormat="1" ht="16" thickBot="1">
@@ -4160,7 +4171,7 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="76"/>
-      <c r="C9" s="173" t="s">
+      <c r="C9" s="164" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4203,7 +4214,7 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="76"/>
-      <c r="C13" s="174" t="s">
+      <c r="C13" s="165" t="s">
         <v>140</v>
       </c>
       <c r="D13" s="71" t="s">
@@ -4228,7 +4239,7 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="76"/>
-      <c r="C14" s="174" t="s">
+      <c r="C14" s="165" t="s">
         <v>140</v>
       </c>
       <c r="D14" s="71" t="s">
@@ -4253,7 +4264,7 @@
     </row>
     <row r="15" spans="2:10">
       <c r="B15" s="76"/>
-      <c r="C15" s="174" t="s">
+      <c r="C15" s="165" t="s">
         <v>140</v>
       </c>
       <c r="D15" s="71" t="s">
@@ -4278,7 +4289,7 @@
     </row>
     <row r="16" spans="2:10">
       <c r="B16" s="76"/>
-      <c r="C16" s="174" t="s">
+      <c r="C16" s="165" t="s">
         <v>140</v>
       </c>
       <c r="D16" s="118" t="s">

</xml_diff>